<commit_message>
end of first year
</commit_message>
<xml_diff>
--- a/теория вероятностей/lab1.xlsx
+++ b/теория вероятностей/lab1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\СевГУ\Documents\tvlabs\tv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\Теория вероятностей\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28755" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -240,34 +240,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.7</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -645,34 +645,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.61499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.505</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63</c:v>
+                  <c:v>0.57499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.54500000000000004</c:v>
+                  <c:v>0.58499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58499999999999996</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.59499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.54500000000000004</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.61499999999999999</c:v>
+                  <c:v>0.56499999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2384,7 +2384,7 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+      <selection activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,38 +2471,38 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5.9926917325357829</v>
+        <v>2.5252641376995149</v>
       </c>
       <c r="B2">
-        <v>3.5008847315897089</v>
+        <v>6.0857267983031704</v>
       </c>
       <c r="C2">
-        <v>3.2264134647663809</v>
+        <v>6.7977480391857661</v>
       </c>
       <c r="D2">
-        <v>5.3854686117130042</v>
+        <v>5.839415570543534</v>
       </c>
       <c r="E2">
-        <v>5.1657133701590014</v>
+        <v>7.1509961241492963</v>
       </c>
       <c r="F2">
-        <v>5.9044688253425699</v>
+        <v>4.9145899838251896</v>
       </c>
       <c r="G2">
-        <v>2.3737702566606647</v>
+        <v>6.7426755577257609</v>
       </c>
       <c r="H2">
-        <v>5.5335761589403978</v>
+        <v>6.50064180425428</v>
       </c>
       <c r="I2">
-        <v>2.8355592516861474</v>
+        <v>5.1054722739341409</v>
       </c>
       <c r="J2">
-        <v>5.0119025238807335</v>
+        <v>6.960292062135685</v>
       </c>
       <c r="K2">
         <f>IF(AND(A2&gt;=3.27,A2&lt;=6.69),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <f t="shared" ref="L2:T2" si="0">IF(AND(B2&gt;=3.27,B2&lt;=6.69),1,0)</f>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="O2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
@@ -2534,60 +2534,60 @@
       </c>
       <c r="S2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2">
         <v>1</v>
       </c>
       <c r="W2">
-        <v>0.57999999999999996</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="X2">
         <v>0.58561600000000003</v>
       </c>
       <c r="Y2">
         <f>ABS(W2-X2)</f>
-        <v>5.6160000000000654E-3</v>
+        <v>2.9383999999999966E-2</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5.0778469191564684</v>
+        <v>2.3507788323618275</v>
       </c>
       <c r="B3">
-        <v>3.9701593066194647</v>
+        <v>5.1441477706228831</v>
       </c>
       <c r="C3">
-        <v>3.0399868770409255</v>
+        <v>4.7377877132480855</v>
       </c>
       <c r="D3">
-        <v>1.5792294076357312</v>
+        <v>1.9488744773705253</v>
       </c>
       <c r="E3">
-        <v>2.5826535843989378</v>
+        <v>6.4011905270546583</v>
       </c>
       <c r="F3">
-        <v>2.6232895901364177</v>
+        <v>2.959606006042665</v>
       </c>
       <c r="G3">
-        <v>5.8485052034058649</v>
+        <v>3.6226145207068088</v>
       </c>
       <c r="H3">
-        <v>4.1163063447981196</v>
+        <v>2.4867668691061127</v>
       </c>
       <c r="I3">
-        <v>4.5283697012237925</v>
+        <v>3.0469377727591782</v>
       </c>
       <c r="J3">
-        <v>4.3087926877651297</v>
+        <v>2.0125019074068424</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K21" si="1">IF(AND(A3&gt;=3.27,A3&lt;=6.69),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L21" si="2">IF(AND(B3&gt;=3.27,B3&lt;=6.69),1,0)</f>
@@ -2595,7 +2595,7 @@
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M21" si="3">IF(AND(C3&gt;=3.27,C3&lt;=6.69),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N21" si="4">IF(AND(D3&gt;=3.27,D3&lt;=6.69),1,0)</f>
@@ -2603,7 +2603,7 @@
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O21" si="5">IF(AND(E3&gt;=3.27,E3&lt;=6.69),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P21" si="6">IF(AND(F3&gt;=3.27,F3&lt;=6.69),1,0)</f>
@@ -2615,60 +2615,60 @@
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R21" si="8">IF(AND(H3&gt;=3.27,H3&lt;=6.69),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <f t="shared" ref="S3:S21" si="9">IF(AND(I3&gt;=3.27,I3&lt;=6.69),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T21" si="10">IF(AND(J3&gt;=3.27,J3&lt;=6.69),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3">
         <v>2</v>
       </c>
       <c r="W3">
-        <v>0.505</v>
+        <v>0.54</v>
       </c>
       <c r="X3">
         <v>0.58561600000000003</v>
       </c>
       <c r="Y3">
         <f t="shared" ref="Y3:Y10" si="11">ABS(W3-X3)</f>
-        <v>8.0616000000000021E-2</v>
+        <v>4.561599999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3.9687334818567459</v>
+        <v>6.4257860042115542</v>
       </c>
       <c r="B4">
-        <v>4.7536500137333286</v>
+        <v>5.7918286690878018</v>
       </c>
       <c r="C4">
-        <v>4.0361037018951995</v>
+        <v>4.9488097781304363</v>
       </c>
       <c r="D4">
-        <v>7.2406448561052272</v>
+        <v>6.8587020477919856</v>
       </c>
       <c r="E4">
-        <v>2.8638975188451798</v>
+        <v>3.2699011200292976</v>
       </c>
       <c r="F4">
-        <v>7.2269212927640609</v>
+        <v>3.8462907803582871</v>
       </c>
       <c r="G4">
-        <v>2.5293633838923308</v>
+        <v>6.0267332987456887</v>
       </c>
       <c r="H4">
-        <v>7.2199703970458087</v>
+        <v>6.4140229499191257</v>
       </c>
       <c r="I4">
-        <v>6.1573744926297795</v>
+        <v>7.3335016937772757</v>
       </c>
       <c r="J4">
-        <v>7.1461839655751209</v>
+        <v>2.7312958159123508</v>
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
@@ -2692,19 +2692,19 @@
       </c>
       <c r="P4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <f t="shared" si="10"/>
@@ -2714,58 +2714,58 @@
         <v>3</v>
       </c>
       <c r="W4">
-        <v>0.56999999999999995</v>
+        <v>0.62</v>
       </c>
       <c r="X4">
         <v>0.58561600000000003</v>
       </c>
       <c r="Y4">
         <f t="shared" si="11"/>
-        <v>1.5616000000000074E-2</v>
+        <v>3.438399999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2.491757255775628</v>
+        <v>5.9484911648915064</v>
       </c>
       <c r="B5">
-        <v>2.5705340739158302</v>
+        <v>3.4247813348796043</v>
       </c>
       <c r="C5">
-        <v>4.4736536759544663</v>
+        <v>2.2142561113315224</v>
       </c>
       <c r="D5">
-        <v>2.8485699026459548</v>
+        <v>3.1456761375774409</v>
       </c>
       <c r="E5">
-        <v>1.9237443159276102</v>
+        <v>5.0614499343852044</v>
       </c>
       <c r="F5">
-        <v>5.6583358256782734</v>
+        <v>4.1164845728934596</v>
       </c>
       <c r="G5">
-        <v>2.9328717917416913</v>
+        <v>2.910949736014893</v>
       </c>
       <c r="H5">
-        <v>7.0807742545854051</v>
+        <v>2.1515198217719047</v>
       </c>
       <c r="I5">
-        <v>3.822586443678091</v>
+        <v>5.7265971861934259</v>
       </c>
       <c r="J5">
-        <v>3.5023105563524277</v>
+        <v>6.1659294412060905</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
@@ -2773,7 +2773,7 @@
       </c>
       <c r="O5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <f t="shared" si="6"/>
@@ -2799,54 +2799,54 @@
         <v>4</v>
       </c>
       <c r="W5">
-        <v>0.56000000000000005</v>
+        <v>0.65</v>
       </c>
       <c r="X5">
         <v>0.58561600000000003</v>
       </c>
       <c r="Y5">
         <f t="shared" si="11"/>
-        <v>2.5615999999999972E-2</v>
+        <v>6.4383999999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2.805973387859737</v>
+        <v>5.0343592638935517</v>
       </c>
       <c r="B6">
-        <v>3.4869829401532026</v>
+        <v>3.1893420209356975</v>
       </c>
       <c r="C6">
-        <v>4.3656474501785336</v>
+        <v>6.3610892056031982</v>
       </c>
       <c r="D6">
-        <v>5.6340968047120574</v>
+        <v>2.7008188116092411</v>
       </c>
       <c r="E6">
-        <v>1.7471202734458449</v>
+        <v>2.741454817346721</v>
       </c>
       <c r="F6">
-        <v>5.0373891415143284</v>
+        <v>6.806837672048097</v>
       </c>
       <c r="G6">
-        <v>2.3215494247260962</v>
+        <v>6.6270055238502152</v>
       </c>
       <c r="H6">
-        <v>4.9140552995391698</v>
+        <v>5.4264610736411631</v>
       </c>
       <c r="I6">
-        <v>4.0341431928464617</v>
+        <v>1.8456804101687674</v>
       </c>
       <c r="J6">
-        <v>6.5227420880764182</v>
+        <v>4.1786861781670579</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
@@ -2854,7 +2854,7 @@
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <f t="shared" si="5"/>
@@ -2862,11 +2862,11 @@
       </c>
       <c r="P6">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <f t="shared" si="8"/>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="S6">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <f t="shared" si="10"/>
@@ -2884,46 +2884,46 @@
         <v>5</v>
       </c>
       <c r="W6">
-        <v>0.63</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="X6">
         <v>0.58561600000000003</v>
       </c>
       <c r="Y6">
         <f t="shared" si="11"/>
-        <v>4.4383999999999979E-2</v>
+        <v>1.061600000000007E-2</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5.0511127048554947</v>
+        <v>4.2344715720084229</v>
       </c>
       <c r="B7">
-        <v>6.9813229773857843</v>
+        <v>5.3029490035706655</v>
       </c>
       <c r="C7">
-        <v>5.9493823053682053</v>
+        <v>4.1927661976989041</v>
       </c>
       <c r="D7">
-        <v>5.7745405438398381</v>
+        <v>4.2678002258369698</v>
       </c>
       <c r="E7">
-        <v>3.5383126316110722</v>
+        <v>1.7952418591875974</v>
       </c>
       <c r="F7">
-        <v>6.6057963805047759</v>
+        <v>2.3566603595080418</v>
       </c>
       <c r="G7">
-        <v>6.1336701559495834</v>
+        <v>6.5587441633350627</v>
       </c>
       <c r="H7">
-        <v>2.5391659291360211</v>
+        <v>5.7424594866786709</v>
       </c>
       <c r="I7">
-        <v>2.7788827173680835</v>
+        <v>4.1974001281777396</v>
       </c>
       <c r="J7">
-        <v>2.3773348185674612</v>
+        <v>5.5266252632221438</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
@@ -2931,7 +2931,7 @@
       </c>
       <c r="L7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
@@ -2943,11 +2943,11 @@
       </c>
       <c r="O7">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <f t="shared" si="7"/>
@@ -2955,72 +2955,72 @@
       </c>
       <c r="R7">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <v>6</v>
       </c>
       <c r="W7">
-        <v>0.54500000000000004</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="X7">
         <v>0.58561600000000003</v>
       </c>
       <c r="Y7">
         <f t="shared" si="11"/>
-        <v>4.0615999999999985E-2</v>
+        <v>6.1600000000006094E-4</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6.048120670186468</v>
+        <v>1.8387295144505142</v>
       </c>
       <c r="B8">
-        <v>3.6600424207281712</v>
+        <v>2.8970479445783868</v>
       </c>
       <c r="C8">
-        <v>4.0430545976134526</v>
+        <v>1.5724567400128178</v>
       </c>
       <c r="D8">
-        <v>3.9243546861171303</v>
+        <v>5.6497808771019624</v>
       </c>
       <c r="E8">
-        <v>3.6504181035798213</v>
+        <v>2.4236741233558154</v>
       </c>
       <c r="F8">
-        <v>1.8993270668660542</v>
+        <v>6.7777864925077056</v>
       </c>
       <c r="G8">
-        <v>1.9797079378643148</v>
+        <v>5.9322724082155824</v>
       </c>
       <c r="H8">
-        <v>6.2922931608020258</v>
+        <v>3.5263713492233038</v>
       </c>
       <c r="I8">
-        <v>3.8259727774895476</v>
+        <v>3.4511590929898985</v>
       </c>
       <c r="J8">
-        <v>3.7732172612689601</v>
+        <v>7.2335157322916341</v>
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <f t="shared" si="4"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="O8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8">
         <f t="shared" si="6"/>
@@ -3036,7 +3036,7 @@
       </c>
       <c r="Q8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8">
         <f t="shared" si="8"/>
@@ -3048,56 +3048,56 @@
       </c>
       <c r="T8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8">
         <v>7</v>
       </c>
       <c r="W8">
-        <v>0.58499999999999996</v>
+        <v>0.59</v>
       </c>
       <c r="X8">
         <v>0.58561600000000003</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="11"/>
-        <v>6.1600000000006094E-4</v>
+        <f>ABS(W8-X8)</f>
+        <v>4.3839999999999435E-3</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4.0421634571367528</v>
+        <v>2.2196029541917173</v>
       </c>
       <c r="B9">
-        <v>2.4774990081484423</v>
+        <v>2.7295135349589525</v>
       </c>
       <c r="C9">
-        <v>1.9583205664235359</v>
+        <v>5.1090368358409375</v>
       </c>
       <c r="D9">
-        <v>3.6514874721518602</v>
+        <v>3.0991586046937467</v>
       </c>
       <c r="E9">
-        <v>6.717723624378185</v>
+        <v>4.4966451002533034</v>
       </c>
       <c r="F9">
-        <v>2.9072069460127565</v>
+        <v>2.3801864680928984</v>
       </c>
       <c r="G9">
-        <v>5.0603805658131655</v>
+        <v>5.8408413953062528</v>
       </c>
       <c r="H9">
-        <v>2.8555207983642079</v>
+        <v>2.8679967650379954</v>
       </c>
       <c r="I9">
-        <v>6.1247587511825925</v>
+        <v>2.0911004974517047</v>
       </c>
       <c r="J9">
-        <v>4.3775887325663012</v>
+        <v>4.669348124637593</v>
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <f t="shared" si="2"/>
@@ -3105,15 +3105,15 @@
       </c>
       <c r="M9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <f t="shared" si="6"/>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="S9">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9">
         <f t="shared" si="10"/>
@@ -3139,46 +3139,46 @@
         <v>8</v>
       </c>
       <c r="W9">
-        <v>0.55000000000000004</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="X9">
         <v>0.58561600000000003</v>
       </c>
       <c r="Y9">
         <f t="shared" si="11"/>
-        <v>3.5615999999999981E-2</v>
+        <v>9.3839999999999479E-3</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5.967561571092868</v>
+        <v>3.8664305551316875</v>
       </c>
       <c r="B10">
-        <v>6.0463383892330693</v>
+        <v>6.2607467879268768</v>
       </c>
       <c r="C10">
-        <v>6.6596212652974023</v>
+        <v>3.943425092318491</v>
       </c>
       <c r="D10">
-        <v>5.7239237647633283</v>
+        <v>2.2727149266029847</v>
       </c>
       <c r="E10">
-        <v>4.218074587237159</v>
+        <v>6.4698083437604907</v>
       </c>
       <c r="F10">
-        <v>6.0336841944639428</v>
+        <v>3.3693523972289192</v>
       </c>
       <c r="G10">
-        <v>5.9757600634784991</v>
+        <v>6.8595931882686845</v>
       </c>
       <c r="H10">
-        <v>6.8952388073366491</v>
+        <v>7.1581252479628894</v>
       </c>
       <c r="I10">
-        <v>6.6414419995727405</v>
+        <v>2.7081261635181737</v>
       </c>
       <c r="J10">
-        <v>6.1033713797418132</v>
+        <v>1.7841917172765283</v>
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="N10">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10">
         <f t="shared" si="5"/>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="Q10">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10">
         <f t="shared" si="8"/>
@@ -3214,56 +3214,56 @@
       </c>
       <c r="S10">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10">
         <v>9</v>
       </c>
       <c r="W10">
-        <v>0.54500000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="X10">
         <v>0.58561600000000003</v>
       </c>
       <c r="Y10">
         <f t="shared" si="11"/>
-        <v>4.0615999999999985E-2</v>
+        <v>1.4383999999999952E-2</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1.736070131534776</v>
+        <v>2.4680529190954315</v>
       </c>
       <c r="B11">
-        <v>6.9437168492690811</v>
+        <v>4.1676360362559892</v>
       </c>
       <c r="C11">
-        <v>1.9964613788262582</v>
+        <v>4.1122070986053041</v>
       </c>
       <c r="D11">
-        <v>3.3891357158116397</v>
+        <v>1.5785164952543718</v>
       </c>
       <c r="E11">
-        <v>4.2637009796441543</v>
+        <v>6.2689452803125096</v>
       </c>
       <c r="F11">
-        <v>1.8444328135013888</v>
+        <v>1.8396206549272134</v>
       </c>
       <c r="G11">
-        <v>6.2051396221808526</v>
+        <v>3.9133045442060608</v>
       </c>
       <c r="H11">
-        <v>5.7474498733481854</v>
+        <v>4.4813174840540784</v>
       </c>
       <c r="I11">
-        <v>7.0916461684011347</v>
+        <v>1.6494512771996217</v>
       </c>
       <c r="J11">
-        <v>3.4962508011108739</v>
+        <v>5.4505218665120392</v>
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
@@ -3271,15 +3271,15 @@
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <f t="shared" si="5"/>
@@ -3309,50 +3309,50 @@
         <v>10</v>
       </c>
       <c r="W11">
-        <v>0.61499999999999999</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="X11">
         <v>0.58561600000000003</v>
       </c>
       <c r="Y11">
         <f>ABS(W11-X11)</f>
-        <v>2.9383999999999966E-2</v>
+        <v>2.0616000000000079E-2</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3.1579738761558884</v>
+        <v>6.0866179387798702</v>
       </c>
       <c r="B12">
-        <v>5.66172215948973</v>
+        <v>6.314928128910184</v>
       </c>
       <c r="C12">
-        <v>4.6541987365337079</v>
+        <v>4.1795773186437577</v>
       </c>
       <c r="D12">
-        <v>4.8958760338145089</v>
+        <v>2.979745780816065</v>
       </c>
       <c r="E12">
-        <v>6.1229764702291938</v>
+        <v>3.9450291451765498</v>
       </c>
       <c r="F12">
-        <v>6.9954029969176306</v>
+        <v>6.4628574480422367</v>
       </c>
       <c r="G12">
-        <v>3.2841593676564838</v>
+        <v>4.7379659413434245</v>
       </c>
       <c r="H12">
-        <v>6.2792825098422185</v>
+        <v>5.0618063905758843</v>
       </c>
       <c r="I12">
-        <v>6.3311468855861079</v>
+        <v>7.0166121402630699</v>
       </c>
       <c r="J12">
-        <v>4.7597097689748837</v>
+        <v>6.8105804620502335</v>
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
@@ -3364,7 +3364,7 @@
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <f t="shared" si="5"/>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="P12">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
         <f t="shared" si="7"/>
@@ -3384,70 +3384,70 @@
       </c>
       <c r="S12">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X12" t="s">
         <v>24</v>
       </c>
       <c r="Y12">
         <f>MAX(Y2:Y11)</f>
-        <v>8.0616000000000021E-2</v>
+        <v>6.4383999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3.7956740012817773</v>
+        <v>2.6218637653736989</v>
       </c>
       <c r="B13">
-        <v>3.8612619403668322</v>
+        <v>1.8643943601794488</v>
       </c>
       <c r="C13">
-        <v>4.5668669698171938</v>
+        <v>1.7756367687002168</v>
       </c>
       <c r="D13">
-        <v>2.032819910275582</v>
+        <v>4.7192519913327438</v>
       </c>
       <c r="E13">
-        <v>6.9371224097415078</v>
+        <v>3.9945765556810207</v>
       </c>
       <c r="F13">
-        <v>3.4069585253456225</v>
+        <v>6.4398660237433996</v>
       </c>
       <c r="G13">
-        <v>3.3048338267159032</v>
+        <v>3.3631144138920255</v>
       </c>
       <c r="H13">
-        <v>5.0821243934446239</v>
+        <v>5.0372109134189884</v>
       </c>
       <c r="I13">
-        <v>2.475538499099704</v>
+        <v>4.1000875881221965</v>
       </c>
       <c r="J13">
-        <v>6.9872045045319977</v>
+        <v>6.6074004333628347</v>
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13">
         <f t="shared" si="6"/>
@@ -3463,11 +3463,11 @@
       </c>
       <c r="S13">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T13">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X13" t="s">
         <v>25</v>
@@ -3479,42 +3479,42 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3.3734516434217356</v>
+        <v>2.1050022888882109</v>
       </c>
       <c r="B14">
-        <v>4.9001535081026644</v>
+        <v>3.1510229804376353</v>
       </c>
       <c r="C14">
-        <v>4.8775185399945071</v>
+        <v>3.8003079317606128</v>
       </c>
       <c r="D14">
-        <v>5.9493823053682053</v>
+        <v>6.5929639576403085</v>
       </c>
       <c r="E14">
-        <v>5.330574358348338</v>
+        <v>2.8458964812158571</v>
       </c>
       <c r="F14">
-        <v>3.0100445570238348</v>
+        <v>4.9595034638508251</v>
       </c>
       <c r="G14">
-        <v>2.9043552964873198</v>
+        <v>2.9464171269875177</v>
       </c>
       <c r="H14">
-        <v>4.37919278542436</v>
+        <v>3.847360148930326</v>
       </c>
       <c r="I14">
-        <v>6.9718768883327735</v>
+        <v>1.7856175420392468</v>
       </c>
       <c r="J14">
-        <v>2.149381084627827</v>
+        <v>6.5696160771507914</v>
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <f t="shared" si="3"/>
@@ -3526,11 +3526,11 @@
       </c>
       <c r="O14">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <f t="shared" si="7"/>
@@ -3546,55 +3546,55 @@
       </c>
       <c r="T14">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2.8884929960020753</v>
+        <v>3.6153071687978757</v>
       </c>
       <c r="B15">
-        <v>6.8016690572832417</v>
+        <v>6.3430881679738755</v>
       </c>
       <c r="C15">
-        <v>2.9948951689199497</v>
+        <v>5.3950929288613549</v>
       </c>
       <c r="D15">
-        <v>2.1682732627338481</v>
+        <v>5.4421451460310681</v>
       </c>
       <c r="E15">
-        <v>3.8117145298623614</v>
+        <v>6.6059746086001159</v>
       </c>
       <c r="F15">
-        <v>6.0764589373454996</v>
+        <v>5.8572383800775167</v>
       </c>
       <c r="G15">
-        <v>1.6020426038392286</v>
+        <v>6.1803659169286167</v>
       </c>
       <c r="H15">
-        <v>3.5112219611194186</v>
+        <v>6.6662157048249755</v>
       </c>
       <c r="I15">
-        <v>2.1877001251258887</v>
+        <v>5.0272301400799586</v>
       </c>
       <c r="J15">
-        <v>4.5221317178868983</v>
+        <v>6.6981185338908045</v>
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <f t="shared" si="5"/>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="Q15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15">
         <f t="shared" si="8"/>
@@ -3614,51 +3614,51 @@
       </c>
       <c r="S15">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>5.6635044404431278</v>
+        <v>2.3518482009338664</v>
       </c>
       <c r="B16">
-        <v>6.0572103030487989</v>
+        <v>2.6439640491958372</v>
       </c>
       <c r="C16">
-        <v>5.0316858424634541</v>
+        <v>5.089253517258217</v>
       </c>
       <c r="D16">
-        <v>4.9349079866939292</v>
+        <v>2.0208786278878139</v>
       </c>
       <c r="E16">
-        <v>2.4227829828791161</v>
+        <v>5.3672893459883415</v>
       </c>
       <c r="F16">
-        <v>5.6904168828394415</v>
+        <v>6.6733448286385695</v>
       </c>
       <c r="G16">
-        <v>2.9189700003051851</v>
+        <v>2.0110760826441236</v>
       </c>
       <c r="H16">
-        <v>4.5429844050416577</v>
+        <v>3.0344618060853907</v>
       </c>
       <c r="I16">
-        <v>2.8118549150059513</v>
+        <v>5.6018375194555494</v>
       </c>
       <c r="J16">
-        <v>5.573142796105838</v>
+        <v>1.9037827692495499</v>
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16">
         <f t="shared" si="3"/>
@@ -3666,11 +3666,11 @@
       </c>
       <c r="N16">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16">
         <f t="shared" si="6"/>
@@ -3682,47 +3682,47 @@
       </c>
       <c r="R16">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4.0574910733359779</v>
+        <v>5.3977663502914517</v>
       </c>
       <c r="B17">
-        <v>4.4818521683400983</v>
+        <v>1.5610501419110692</v>
       </c>
       <c r="C17">
-        <v>4.9885546433912173</v>
+        <v>3.6388332773827328</v>
       </c>
       <c r="D17">
-        <v>3.6135248878444779</v>
+        <v>2.9551503036591695</v>
       </c>
       <c r="E17">
-        <v>5.4521259193700979</v>
+        <v>6.9581533249916072</v>
       </c>
       <c r="F17">
-        <v>3.5878600421155431</v>
+        <v>6.291223792229987</v>
       </c>
       <c r="G17">
-        <v>4.9302740562150946</v>
+        <v>7.3545326090273742</v>
       </c>
       <c r="H17">
-        <v>2.3015878780480361</v>
+        <v>4.0760267952513196</v>
       </c>
       <c r="I17">
-        <v>2.0878923917355876</v>
+        <v>2.4368630024109623</v>
       </c>
       <c r="J17">
-        <v>6.6198764000366221</v>
+        <v>3.9976064333017973</v>
       </c>
       <c r="K17">
         <f t="shared" si="1"/>
@@ -3730,7 +3730,7 @@
       </c>
       <c r="L17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17">
         <f t="shared" si="3"/>
@@ -3738,11 +3738,11 @@
       </c>
       <c r="N17">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17">
         <f t="shared" si="6"/>
@@ -3750,11 +3750,11 @@
       </c>
       <c r="Q17">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17">
         <f t="shared" si="9"/>
@@ -3767,46 +3767,46 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>4.6178402050843834</v>
+        <v>3.0057670827356793</v>
       </c>
       <c r="B18">
-        <v>2.4049601733451338</v>
+        <v>5.2874431592761013</v>
       </c>
       <c r="C18">
-        <v>3.652735068819239</v>
+        <v>7.3541761528366951</v>
       </c>
       <c r="D18">
-        <v>4.0218454542680133</v>
+        <v>3.5705719168675802</v>
       </c>
       <c r="E18">
-        <v>6.3156410412915429</v>
+        <v>4.8967671742912078</v>
       </c>
       <c r="F18">
-        <v>3.3378060243537706</v>
+        <v>7.1948402356028929</v>
       </c>
       <c r="G18">
-        <v>2.0411966307565539</v>
+        <v>3.2208883938108461</v>
       </c>
       <c r="H18">
-        <v>5.9010824915311133</v>
+        <v>2.4548640400402846</v>
       </c>
       <c r="I18">
-        <v>1.8909503463850825</v>
+        <v>4.9554042176580095</v>
       </c>
       <c r="J18">
-        <v>6.7337641529587691</v>
+        <v>2.3871373638111515</v>
       </c>
       <c r="K18">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18">
         <f t="shared" si="4"/>
@@ -3818,7 +3818,7 @@
       </c>
       <c r="P18">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18">
         <f t="shared" si="7"/>
@@ -3826,11 +3826,11 @@
       </c>
       <c r="R18">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18">
         <f t="shared" si="10"/>
@@ -3839,34 +3839,34 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5.1635746330149228</v>
+        <v>4.9498791467024752</v>
       </c>
       <c r="B19">
-        <v>5.5701129184850604</v>
+        <v>4.153377788628803</v>
       </c>
       <c r="C19">
-        <v>4.0738880581072419</v>
+        <v>2.7127600939970091</v>
       </c>
       <c r="D19">
-        <v>5.1582277901547284</v>
+        <v>5.9508081301309241</v>
       </c>
       <c r="E19">
-        <v>4.3816879787591176</v>
+        <v>5.0864018677327802</v>
       </c>
       <c r="F19">
-        <v>2.0506427198095647</v>
+        <v>2.2996273689992979</v>
       </c>
       <c r="G19">
-        <v>5.9586501663258762</v>
+        <v>7.0977059236426889</v>
       </c>
       <c r="H19">
-        <v>5.0495086519974359</v>
+        <v>7.0144734031189913</v>
       </c>
       <c r="I19">
-        <v>2.7740705587939085</v>
+        <v>3.0988021485030672</v>
       </c>
       <c r="J19">
-        <v>3.6067522202215638</v>
+        <v>1.5596243171483506</v>
       </c>
       <c r="K19">
         <f t="shared" si="1"/>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="M19">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19">
         <f t="shared" si="4"/>
@@ -3894,11 +3894,11 @@
       </c>
       <c r="Q19">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S19">
         <f t="shared" si="9"/>
@@ -3906,47 +3906,47 @@
       </c>
       <c r="T19">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>3.2536823633533736</v>
+        <v>3.6571907712027345</v>
       </c>
       <c r="B20">
-        <v>1.5826157414471878</v>
+        <v>6.4952949613940856</v>
       </c>
       <c r="C20">
-        <v>6.5942115543076874</v>
+        <v>3.8361317789239173</v>
       </c>
       <c r="D20">
-        <v>7.3821579638050476</v>
+        <v>2.5489684743797114</v>
       </c>
       <c r="E20">
-        <v>6.4580452894680622</v>
+        <v>6.3812289803765987</v>
       </c>
       <c r="F20">
-        <v>7.1096472060304574</v>
+        <v>5.4412540055543692</v>
       </c>
       <c r="G20">
-        <v>2.0010953093050934</v>
+        <v>6.5074144718771931</v>
       </c>
       <c r="H20">
-        <v>5.6946943571275979</v>
+        <v>3.5030234687337867</v>
       </c>
       <c r="I20">
-        <v>2.2687939085055087</v>
+        <v>6.6950886562700278</v>
       </c>
       <c r="J20">
-        <v>4.145535752433851</v>
+        <v>4.0164986114078189</v>
       </c>
       <c r="K20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20">
         <f t="shared" si="3"/>
@@ -3962,11 +3962,11 @@
       </c>
       <c r="P20">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20">
         <f t="shared" si="8"/>
@@ -3983,42 +3983,42 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>6.3099377422406686</v>
+        <v>2.6143781853694268</v>
       </c>
       <c r="B21">
-        <v>2.3796517838068789</v>
+        <v>4.2882964568010502</v>
       </c>
       <c r="C21">
-        <v>1.6421439252906889</v>
+        <v>3.0408780175176244</v>
       </c>
       <c r="D21">
-        <v>6.3159974974822228</v>
+        <v>4.0125775933103425</v>
       </c>
       <c r="E21">
-        <v>5.5989858699301118</v>
+        <v>4.1927661976989041</v>
       </c>
       <c r="F21">
-        <v>2.1336970122379224</v>
+        <v>7.0923590807824946</v>
       </c>
       <c r="G21">
-        <v>5.330752586443678</v>
+        <v>5.3745966978972746</v>
       </c>
       <c r="H21">
-        <v>4.7971376689962462</v>
+        <v>4.8443681142612993</v>
       </c>
       <c r="I21">
-        <v>2.2411685537278361</v>
+        <v>3.9894079409161654</v>
       </c>
       <c r="J21">
-        <v>2.9735077974791713</v>
+        <v>5.2184688863795889</v>
       </c>
       <c r="K21">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21">
         <f t="shared" si="3"/>
@@ -4046,11 +4046,11 @@
       </c>
       <c r="S21">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -4059,19 +4059,19 @@
       </c>
       <c r="K22">
         <f>SUM(K2:K21)/20</f>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="L22">
         <f t="shared" ref="L22:T22" si="12">SUM(L2:L21)/20</f>
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="M22">
         <f t="shared" si="12"/>
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="N22">
         <f t="shared" si="12"/>
-        <v>0.7</v>
+        <v>0.45</v>
       </c>
       <c r="O22">
         <f t="shared" si="12"/>
@@ -4079,27 +4079,27 @@
       </c>
       <c r="P22">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q22">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="R22">
-        <f t="shared" si="12"/>
-        <v>0.7</v>
+        <f>SUM(R2:R21)/20</f>
+        <v>0.65</v>
       </c>
       <c r="S22">
         <f t="shared" si="12"/>
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="T22">
         <f t="shared" si="12"/>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="U22">
         <f>AVERAGE(K22:T22)</f>
-        <v>0.61499999999999999</v>
+        <v>0.56500000000000006</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>